<commit_message>
feat: Update TB_REG for V2.33 translations
</commit_message>
<xml_diff>
--- a/metadata/TB_Tracker/TB-REG_TRACKER_V1_DHIS2.33/reference.xlsx
+++ b/metadata/TB_Tracker/TB-REG_TRACKER_V1_DHIS2.33/reference.xlsx
@@ -498,7 +498,7 @@
         <v>Created</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>2020-10-10T10:24</v>
+        <v>2020-10-10T12:36</v>
       </c>
     </row>
     <row r="7">
@@ -506,7 +506,7 @@
         <v>Identifier</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>TB-REG_TRACKER_V1.1.0_DHIS2.33_2020-10-10T10:24</v>
+        <v>TB-REG_TRACKER_V1.1.0_DHIS2.33_2020-10-10T12:36</v>
       </c>
     </row>
   </sheetData>
@@ -770,7 +770,7 @@
         <v>Subsequent DST in Liquid Media - Am</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>a4PpEfSutcV</v>
@@ -784,7 +784,7 @@
         <v>Initial DST in Solid Media - Z</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D3" s="5" t="str">
         <v>aCaNdqUIDZl</v>
@@ -798,7 +798,7 @@
         <v>Ethambutol Result</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>2020-08-13</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D4" s="4" t="str">
         <v>AiyTLOJHMkl</v>
@@ -812,7 +812,7 @@
         <v>Initial DST in Solid Media - H CB</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D5" s="5" t="str">
         <v>anpSc1tmlft</v>
@@ -826,7 +826,7 @@
         <v>Initial DST in Liquid Media - Lzd</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D6" s="4" t="str">
         <v>aZq11UuXPP6</v>
@@ -840,7 +840,7 @@
         <v>Subsequent DST in Liquid Media - Lfx</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D7" s="5" t="str">
         <v>b1KgVOel21P</v>
@@ -854,7 +854,7 @@
         <v>Subsequent DST in Solid Media - Z</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D8" s="4" t="str">
         <v>bHPYGfrFNV2</v>
@@ -868,7 +868,7 @@
         <v>Initial DST in Liquid Media - Dlm</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D9" s="5" t="str">
         <v>BJTzi3WWjhT</v>
@@ -896,7 +896,7 @@
         <v>Subsequent DST in Solid Media - Cfz</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D11" s="5" t="str">
         <v>bywBn5DxVdi</v>
@@ -924,7 +924,7 @@
         <v>Initial DST in Liquid Media - H CC</v>
       </c>
       <c r="C13" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D13" s="5" t="str">
         <v>cRldkiBh5xv</v>
@@ -938,7 +938,7 @@
         <v>Initial DST in Solid Media - Lzd</v>
       </c>
       <c r="C14" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D14" s="4" t="str">
         <v>CVQR2ZtZWxk</v>
@@ -952,7 +952,7 @@
         <v>Subsequent DST in Solid Media - Mfx CC</v>
       </c>
       <c r="C15" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D15" s="5" t="str">
         <v>Czx5FuOqF9i</v>
@@ -966,7 +966,7 @@
         <v>Initial DST in Solid Media - H CC</v>
       </c>
       <c r="C16" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D16" s="4" t="str">
         <v>dAPAScvFPfX</v>
@@ -980,7 +980,7 @@
         <v>Initial DST in Liquid Media - Mfx CC</v>
       </c>
       <c r="C17" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D17" s="5" t="str">
         <v>dgjpdQO2Iva</v>
@@ -994,7 +994,7 @@
         <v>Subsequent DST in Solid Media - Am</v>
       </c>
       <c r="C18" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D18" s="4" t="str">
         <v>dTwKm1u2VhY</v>
@@ -1008,7 +1008,7 @@
         <v>Subsequent DST in Solid Media - H CC</v>
       </c>
       <c r="C19" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D19" s="5" t="str">
         <v>eM3UfUO7W8O</v>
@@ -1036,7 +1036,7 @@
         <v>Subsequent DST in Liquid Media - H CB</v>
       </c>
       <c r="C21" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D21" s="5" t="str">
         <v>F9DTb5zl8rS</v>
@@ -1050,7 +1050,7 @@
         <v>Initial DST in Liquid Media - Z</v>
       </c>
       <c r="C22" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D22" s="4" t="str">
         <v>FDtk4otxDse</v>
@@ -1064,7 +1064,7 @@
         <v>Subsequent DST in Solid Media - Lfx</v>
       </c>
       <c r="C23" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D23" s="5" t="str">
         <v>Fw8wOlTETPt</v>
@@ -1078,7 +1078,7 @@
         <v>Initial DST in Liquid Media - Cfz</v>
       </c>
       <c r="C24" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D24" s="4" t="str">
         <v>GL5JTtBvbEC</v>
@@ -1134,7 +1134,7 @@
         <v>Subsequent DST in Liquid Media - Mfx CC</v>
       </c>
       <c r="C28" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D28" s="4" t="str">
         <v>HhKitGif8RV</v>
@@ -1162,7 +1162,7 @@
         <v>Subsequent DST in Liquid Media - E</v>
       </c>
       <c r="C30" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D30" s="4" t="str">
         <v>Ic5asMdbpH8</v>
@@ -1190,7 +1190,7 @@
         <v>Subsequent DST in Solid Media - Lzd</v>
       </c>
       <c r="C32" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D32" s="4" t="str">
         <v>KIeI2d8xalG</v>
@@ -1204,7 +1204,7 @@
         <v>Initial DST in Liquid Media - Bdq</v>
       </c>
       <c r="C33" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D33" s="5" t="str">
         <v>KjvwSybuWJU</v>
@@ -1218,7 +1218,7 @@
         <v>Subsequent DST in Liquid Media - R</v>
       </c>
       <c r="C34" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D34" s="4" t="str">
         <v>lelJEADYpeI</v>
@@ -1232,7 +1232,7 @@
         <v>Initial DST in Liquid Media - H CB</v>
       </c>
       <c r="C35" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D35" s="5" t="str">
         <v>lqaf0KfpHGd</v>
@@ -1246,7 +1246,7 @@
         <v>Initial DST in Solid Media - Mfx CB</v>
       </c>
       <c r="C36" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D36" s="4" t="str">
         <v>m4c79OHEKCG</v>
@@ -1260,7 +1260,7 @@
         <v>Subsequent DST in Liquid Media - Lzd</v>
       </c>
       <c r="C37" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D37" s="5" t="str">
         <v>mU5iEABeF2K</v>
@@ -1274,7 +1274,7 @@
         <v>Initial DST in Liquid Media - E</v>
       </c>
       <c r="C38" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D38" s="4" t="str">
         <v>n9zOOsLO0QP</v>
@@ -1288,7 +1288,7 @@
         <v>Subsequent DST in Liquid Media - Cfz</v>
       </c>
       <c r="C39" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D39" s="5" t="str">
         <v>Nb6oHqjCCZq</v>
@@ -1302,7 +1302,7 @@
         <v>Initial DST in Solid Media - Lfx</v>
       </c>
       <c r="C40" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D40" s="4" t="str">
         <v>NlOX3oV4gWe</v>
@@ -1316,7 +1316,7 @@
         <v>Subsequent DST in Solid Media - Mfx CB</v>
       </c>
       <c r="C41" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D41" s="5" t="str">
         <v>NvA1K4hFJbc</v>
@@ -1358,7 +1358,7 @@
         <v>Initial DST in Solid Media - R</v>
       </c>
       <c r="C44" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D44" s="4" t="str">
         <v>Q67DDsupq7v</v>
@@ -1372,7 +1372,7 @@
         <v>Subsequent DST in Liquid Media - Bdq</v>
       </c>
       <c r="C45" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D45" s="5" t="str">
         <v>QaioqMbO0TX</v>
@@ -1400,7 +1400,7 @@
         <v>Subsequent DST in Solid Media - Bdq</v>
       </c>
       <c r="C47" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D47" s="5" t="str">
         <v>r70ONQRhaHY</v>
@@ -1414,7 +1414,7 @@
         <v>Subsequent DST in Solid Media - Dlm</v>
       </c>
       <c r="C48" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D48" s="4" t="str">
         <v>RFqmLP5W5di</v>
@@ -1442,7 +1442,7 @@
         <v>Initial DST in Solid Media - Mfx CC</v>
       </c>
       <c r="C50" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D50" s="4" t="str">
         <v>RJNE1o9cw7Y</v>
@@ -1456,7 +1456,7 @@
         <v>Subsequent DST in Solid Media - H CB</v>
       </c>
       <c r="C51" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D51" s="5" t="str">
         <v>s8WPR943gGS</v>
@@ -1470,7 +1470,7 @@
         <v>Initial DST in Liquid Media - Lfx</v>
       </c>
       <c r="C52" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D52" s="4" t="str">
         <v>t7Okdm8VgDV</v>
@@ -1484,7 +1484,7 @@
         <v>Initial DST in Liquid Media - Mfx CB</v>
       </c>
       <c r="C53" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D53" s="5" t="str">
         <v>UL61U78GWCg</v>
@@ -1498,7 +1498,7 @@
         <v>Initial DST in Liquid Media - R</v>
       </c>
       <c r="C54" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D54" s="4" t="str">
         <v>uOJYEwV7XfN</v>
@@ -1512,7 +1512,7 @@
         <v>Initial DST in Solid Media - Bdq</v>
       </c>
       <c r="C55" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D55" s="5" t="str">
         <v>UxcTzMRQsfa</v>
@@ -1526,7 +1526,7 @@
         <v>Initial DST in Solid Media - Dlm</v>
       </c>
       <c r="C56" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D56" s="4" t="str">
         <v>VUlsMrm4D8k</v>
@@ -1540,7 +1540,7 @@
         <v>Subsequent DST in Liquid Media - Z</v>
       </c>
       <c r="C57" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D57" s="5" t="str">
         <v>VY15auehssY</v>
@@ -1568,7 +1568,7 @@
         <v>Subsequent DST in Solid Media - E</v>
       </c>
       <c r="C59" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D59" s="5" t="str">
         <v>wNxsAieLWYc</v>
@@ -1582,7 +1582,7 @@
         <v>Initial DST in Liquid Media - Am</v>
       </c>
       <c r="C60" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D60" s="4" t="str">
         <v>x6v8O6EZo0U</v>
@@ -1596,7 +1596,7 @@
         <v>Subsequent DST in Liquid Media - Mfx CB</v>
       </c>
       <c r="C61" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D61" s="5" t="str">
         <v>xfltmyqC3p0</v>
@@ -1610,7 +1610,7 @@
         <v>Initial DST in Solid Media - Am</v>
       </c>
       <c r="C62" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D62" s="4" t="str">
         <v>XO1V9o5C95J</v>
@@ -1624,7 +1624,7 @@
         <v>Subsequent DST in Liquid Media - Dlm</v>
       </c>
       <c r="C63" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D63" s="5" t="str">
         <v>Xt5GU9kBD7q</v>
@@ -1652,7 +1652,7 @@
         <v>Initial DST in Solid Media - E</v>
       </c>
       <c r="C65" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D65" s="5" t="str">
         <v>yxPHZFwMTN6</v>
@@ -1680,7 +1680,7 @@
         <v>Subsequent DST in Liquid Media - H CC</v>
       </c>
       <c r="C67" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D67" s="5" t="str">
         <v>ZBpqH7xJLBO</v>
@@ -1694,7 +1694,7 @@
         <v>Initial DST in Solid Media - Cfz</v>
       </c>
       <c r="C68" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D68" s="4" t="str">
         <v>ZDpLleSK08x</v>
@@ -1708,7 +1708,7 @@
         <v>Subsequent DST in Solid Media - R</v>
       </c>
       <c r="C69" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="D69" s="5" t="str">
         <v>zJoEjvstp2d</v>
@@ -2050,7 +2050,7 @@
         <v>default</v>
       </c>
       <c r="F14" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G14" s="4" t="str">
         <v>BNkkWpCKgLR</v>
@@ -2073,7 +2073,7 @@
         <v>default</v>
       </c>
       <c r="F15" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G15" s="5" t="str">
         <v>bXaGYMAnfNH</v>
@@ -2303,7 +2303,7 @@
         <v>default</v>
       </c>
       <c r="F25" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G25" s="5" t="str">
         <v>Dd95Kl4aXZf</v>
@@ -2349,7 +2349,7 @@
         <v>default</v>
       </c>
       <c r="F27" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G27" s="5" t="str">
         <v>DjVjz7PNXJA</v>
@@ -2464,7 +2464,7 @@
         <v>default</v>
       </c>
       <c r="F32" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G32" s="4" t="str">
         <v>E61DoZgoPH2</v>
@@ -2579,7 +2579,7 @@
         <v>default</v>
       </c>
       <c r="F37" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G37" s="5" t="str">
         <v>ema8JjkIDTz</v>
@@ -2740,7 +2740,7 @@
         <v>default</v>
       </c>
       <c r="F44" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G44" s="4" t="str">
         <v>FjsunwwqBMk</v>
@@ -2763,7 +2763,7 @@
         <v>default</v>
       </c>
       <c r="F45" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G45" s="5" t="str">
         <v>FKxBceeFNuR</v>
@@ -2924,7 +2924,7 @@
         <v>default</v>
       </c>
       <c r="F52" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G52" s="4" t="str">
         <v>HkZ1hGWBqlZ</v>
@@ -2993,7 +2993,7 @@
         <v>default</v>
       </c>
       <c r="F55" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G55" s="5" t="str">
         <v>IBqX2HMQV4T</v>
@@ -3246,7 +3246,7 @@
         <v>default</v>
       </c>
       <c r="F66" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G66" s="4" t="str">
         <v>jC2yaMqEOPb</v>
@@ -3269,7 +3269,7 @@
         <v>default</v>
       </c>
       <c r="F67" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G67" s="5" t="str">
         <v>jD5CwNpVmb3</v>
@@ -3752,7 +3752,7 @@
         <v>default</v>
       </c>
       <c r="F88" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G88" s="4" t="str">
         <v>nBVHqtynKKg</v>
@@ -3867,7 +3867,7 @@
         <v>default</v>
       </c>
       <c r="F93" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G93" s="5" t="str">
         <v>oKdArKmQaar</v>
@@ -3959,7 +3959,7 @@
         <v>default</v>
       </c>
       <c r="F97" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G97" s="5" t="str">
         <v>OXN8xMgpVvC</v>
@@ -3982,7 +3982,7 @@
         <v>default</v>
       </c>
       <c r="F98" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G98" s="4" t="str">
         <v>OZV3tzf7bux</v>
@@ -4028,7 +4028,7 @@
         <v>default</v>
       </c>
       <c r="F100" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G100" s="4" t="str">
         <v>p3L4HYkzU4o</v>
@@ -4051,7 +4051,7 @@
         <v>default</v>
       </c>
       <c r="F101" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G101" s="5" t="str">
         <v>peAahjwkqNX</v>
@@ -4143,7 +4143,7 @@
         <v>default</v>
       </c>
       <c r="F105" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G105" s="5" t="str">
         <v>pXViXBpKM6Y</v>
@@ -4235,7 +4235,7 @@
         <v>default</v>
       </c>
       <c r="F109" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G109" s="5" t="str">
         <v>QQEolquguCi</v>
@@ -4258,7 +4258,7 @@
         <v>default</v>
       </c>
       <c r="F110" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G110" s="4" t="str">
         <v>qt2LpZN8Hb3</v>
@@ -4350,7 +4350,7 @@
         <v>default</v>
       </c>
       <c r="F114" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G114" s="4" t="str">
         <v>RAtv78ZXQec</v>
@@ -4695,7 +4695,7 @@
         <v>default</v>
       </c>
       <c r="F129" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G129" s="5" t="str">
         <v>uaewAATQgBJ</v>
@@ -4741,7 +4741,7 @@
         <v>default</v>
       </c>
       <c r="F131" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G131" s="5" t="str">
         <v>uEV8flIOeYI</v>
@@ -4810,7 +4810,7 @@
         <v>default</v>
       </c>
       <c r="F134" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G134" s="4" t="str">
         <v>uI7p5xLE1C8</v>
@@ -5109,7 +5109,7 @@
         <v>default</v>
       </c>
       <c r="F147" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G147" s="5" t="str">
         <v>Wg7Df5kgpaF</v>
@@ -5155,7 +5155,7 @@
         <v>default</v>
       </c>
       <c r="F149" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G149" s="5" t="str">
         <v>wi4NRarMSuv</v>
@@ -5477,7 +5477,7 @@
         <v>default</v>
       </c>
       <c r="F163" s="5" t="str">
-        <v>2020-08-13</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G163" s="5" t="str">
         <v>yiGr4JTFLv3</v>
@@ -5615,7 +5615,7 @@
         <v>default</v>
       </c>
       <c r="F169" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="G169" s="5" t="str">
         <v>zcmsN575vwZ</v>
@@ -7117,7 +7117,7 @@
         <v>default</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>bjDvmb4bfuf</v>
@@ -7162,7 +7162,7 @@
         <v>default</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-10-08</v>
+        <v>2020-10-10</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>GLevLNI9wkl</v>
@@ -7203,7 +7203,7 @@
         <v>default</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>xYerKDKCefk</v>
@@ -7241,7 +7241,7 @@
         <v>default</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>HllvX50cXC0</v>
@@ -7792,7 +7792,7 @@
         <v>NO_GROWTH</v>
       </c>
       <c r="D18" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E18" s="4" t="str">
         <v>rB88xT5ggFg</v>
@@ -7945,7 +7945,7 @@
         <v>RESISTANT</v>
       </c>
       <c r="D27" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E27" s="5" t="str">
         <v>q75AsvLUWVp</v>
@@ -7979,7 +7979,7 @@
         <v>SUSCEPTIBLE</v>
       </c>
       <c r="D29" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E29" s="5" t="str">
         <v>q75AsvLUWVp</v>
@@ -7996,7 +7996,7 @@
         <v>NO</v>
       </c>
       <c r="D30" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E30" s="4" t="str">
         <v>bLA3AqDKdwx</v>
@@ -8064,7 +8064,7 @@
         <v>HISTORY_FAILED</v>
       </c>
       <c r="D34" s="4" t="str">
-        <v>2020-08-04</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E34" s="4" t="str">
         <v>cEiPBSWUO5S</v>
@@ -8098,7 +8098,7 @@
         <v>RESISTANT</v>
       </c>
       <c r="D36" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E36" s="4" t="str">
         <v>ekhfzhURD44</v>
@@ -8323,7 +8323,7 @@
         <v>Person</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-08-13</v>
+        <v>2020-10-10</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>MCPQUTHX1Ze</v>
@@ -12830,7 +12830,7 @@
         <v>Family name of the patient</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>2020-08-13</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E2" s="4" t="str">
         <v>aW66s2QSosT</v>
@@ -12847,7 +12847,7 @@
         <v/>
       </c>
       <c r="D3" s="5" t="str">
-        <v>2020-08-04</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E3" s="5" t="str">
         <v>ciCR6BBvIT4</v>
@@ -12915,7 +12915,7 @@
         <v>Date of birth plus calculated age</v>
       </c>
       <c r="D7" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E7" s="5" t="str">
         <v>mAWcalQYYyk</v>
@@ -12949,7 +12949,7 @@
         <v>The name of the patient or initials</v>
       </c>
       <c r="D9" s="5" t="str">
-        <v>2020-08-13</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E9" s="5" t="str">
         <v>TfdH5KvFmMy</v>
@@ -12966,7 +12966,7 @@
         <v>Current home address of the patient</v>
       </c>
       <c r="D10" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E10" s="4" t="str">
         <v>VCtm2pySeEV</v>
@@ -13000,7 +13000,7 @@
         <v/>
       </c>
       <c r="D12" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="E12" s="4" t="str">
         <v>Z1rLc1rVHK8</v>
@@ -15685,7 +15685,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G24" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H24" s="4" t="str">
         <v>Lt6P15ps7f6</v>
@@ -16569,7 +16569,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G58" s="4" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H58" s="4" t="str">
         <v>Lt6P15ps7f6</v>
@@ -18207,7 +18207,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G121" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H121" s="5" t="str">
         <v>Lt6P15ps7f6</v>
@@ -19299,7 +19299,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G163" s="5" t="str">
-        <v>2020-08-04</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H163" s="5" t="str">
         <v>Lt6P15ps7f6</v>
@@ -19793,7 +19793,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G182" s="4" t="str">
-        <v>2020-08-04</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H182" s="4" t="str">
         <v>Lt6P15ps7f6</v>
@@ -19923,7 +19923,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G187" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H187" s="5" t="str">
         <v>Lt6P15ps7f6</v>
@@ -20183,7 +20183,7 @@
         <v>ENROLLMENT</v>
       </c>
       <c r="G197" s="5" t="str">
-        <v>2020-09-24</v>
+        <v>2020-10-10</v>
       </c>
       <c r="H197" s="5" t="str">
         <v>Lt6P15ps7f6</v>

</xml_diff>